<commit_message>
5 bento scripts troubleshooted and working fine in visible and headless
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_2.xlsx
+++ b/InputFiles/TC02_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B84DA58-3E92-4D3F-BA69-13ABACF57257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0427CBC4-3E4A-4C76-83C1-D3B128ED11C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="60" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>WebExcel</t>
   </si>
@@ -61,13 +61,35 @@
   </si>
   <si>
     <t>TC02_Bento_MultiFilter_Diagnosis-Recurrence-TumorSize-Chemo_2_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
+ WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["IV CMF (3 week cycles)"]
+return ss.study_subject_id as `Case ID`,
+       p.program_acronym as `Program Code`,
+        p.program_id as Program_ID,
+       s.study_acronym as `Arm`,
+       ss.disease_subtype as `Diagnosis`,
+       sf.grouped_recurrence_score AS `Recurrence Score`,
+       d.tumor_size_group AS `tumor_size`,
+       d.er_status AS `ER Status`,
+       d.pr_status AS `PR Status`,
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
 MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Paget's Disease"] and sf.grouped_recurrence_score IN ["11-15"]and d.tumor_size_group In ["(1,2]"] and tp.chemotherapy_regimen In ["Dose dense AC followed by a taxane"]
+WHERE ss.disease_subtype IN ["Medullary Carcinoma"] and sf.grouped_recurrence_score IN ["16-20"]and d.tumor_size_group In ["(2,3]"] and tp.chemotherapy_regimen In ["IV CMF (3 week cycles)"]
 WITH ss
 MATCH (ss)-[:study_subject_of_study]-&gt;(s)
 MATCH (s)-[:study_of_program]-&gt;(p)
@@ -80,77 +102,6 @@
 COUNT(DISTINCT samp) AS Samples,
 COUNT(DISTINCT lp) AS Assays,
 COUNT(DISTINCT f) AS Files</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-WITH COLLECT(ss.study_subject_id) AS all_subjects
-MATCH (samp:sample)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-WHERE ss.disease_subtype IN ["Paget's Disease"] and sf.grouped_recurrence_score IN ["11-15"]and d.tumor_size_group In ["(1,2]"] and tp.chemotherapy_regimen In ["Dose dense AC followed by a taxane"]
-WITH
-    distinct lp,
-    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
-    collect(distinct f.file_id) AS files,
-    samp, ss, s, p, all_subjects
-RETURN
- samp.sample_id AS `Sample ID`,
-            ss.study_subject_id AS `Case ID`,
-            p.program_acronym AS `Program Code`,
-            s.study_acronym AS `Arm`,
-            ss.disease_subtype AS `Diagnosis`,
-            samp.tissue_type AS `Tissue Type`,
-            samp.composition AS `Tissue Composition`,
-            samp.sample_anatomic_site AS `Sample Anatomic Site`,
-            samp.method_of_sample_procurement AS `Sample Procurement Method`,
-            lp.test_name as Platform</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-WHERE ss.disease_subtype IN ["Paget's Disease"] and sf.grouped_recurrence_score IN ["11-15"]and d.tumor_size_group In ["(1,2]"] and tp.chemotherapy_regimen In ["Dose dense AC followed by a taxane"]
-RETURN  f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    f.file_size AS `Size`,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`,
-    ss.disease_subtype as `Diagnosis`</t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
- WHERE ss.disease_subtype IN ["Paget's Disease"] and sf.grouped_recurrence_score IN ["11-15"]and d.tumor_size_group In ["(1,2]"] and tp.chemotherapy_regimen In ["Dose dense AC followed by a taxane"]
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`,
-demo.survival_time AS `Survival (days)`</t>
   </si>
 </sst>
 </file>
@@ -522,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -557,10 +508,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -569,15 +520,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -586,15 +537,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>